<commit_message>
fixed the sales car bug
</commit_message>
<xml_diff>
--- a/data/customers.xlsx
+++ b/data/customers.xlsx
@@ -493,7 +493,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Harish@875#</t>
+          <t>Harish@566#</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -541,7 +541,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Swetha@990#</t>
+          <t>Swetha@633#</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -589,7 +589,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Swetha@567#</t>
+          <t>Swetha@202#</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -637,7 +637,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Deepa@061#</t>
+          <t>Deepa@184#</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -685,7 +685,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Rahul@037#</t>
+          <t>Rahul@466#</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -733,7 +733,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Lakshmi@385#</t>
+          <t>Lakshmi@108#</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -781,7 +781,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Sandeep@538#</t>
+          <t>Sandeep@977#</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -829,7 +829,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Preeti@057#</t>
+          <t>Preeti@540#</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -877,7 +877,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Ajay@096#</t>
+          <t>Ajay@522#</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -925,7 +925,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Rina@790#</t>
+          <t>Rina@054#</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -973,7 +973,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Vivek@033#</t>
+          <t>Vivek@854#</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -1021,7 +1021,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Meena@200#</t>
+          <t>Meena@989#</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -1069,7 +1069,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Sahil@683#</t>
+          <t>Sahil@783#</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -1117,7 +1117,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Tanvi@086#</t>
+          <t>Tanvi@342#</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -1165,7 +1165,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Yash@354#</t>
+          <t>Yash@967#</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1213,7 +1213,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Anita@354#</t>
+          <t>Anita@536#</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1261,7 +1261,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Rohit@464#</t>
+          <t>Rohit@836#</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1309,7 +1309,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Kiran@439#</t>
+          <t>Kiran@397#</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1357,7 +1357,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Sunita@277#</t>
+          <t>Sunita@926#</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1405,7 +1405,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Amitabh@752#</t>
+          <t>Amitabh@917#</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1453,7 +1453,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Priya@730#</t>
+          <t>Priya@227#</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1501,7 +1501,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Nitin@171#</t>
+          <t>Nitin@276#</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1549,7 +1549,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Sneha@721#</t>
+          <t>Sneha@137#</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1597,7 +1597,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Arjun@252#</t>
+          <t>Arjun@085#</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1645,7 +1645,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Divya@313#</t>
+          <t>Divya@819#</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">

</xml_diff>